<commit_message>
Charts and styles added
</commit_message>
<xml_diff>
--- a/TestProjects/DISCGraphing.xlsx
+++ b/TestProjects/DISCGraphing.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Dude5th\TestProjects\TestProjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30706B8F-991E-441E-A5E7-B17E9FFF477D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B36E2FF-8DFE-4044-8902-E985C2F49F99}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="7980" xr2:uid="{EA7BB211-2716-4A1F-BA66-D009593DAA90}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="7980" activeTab="2" xr2:uid="{EA7BB211-2716-4A1F-BA66-D009593DAA90}"/>
   </bookViews>
   <sheets>
     <sheet name="Most" sheetId="1" r:id="rId1"/>
+    <sheet name="Least" sheetId="2" r:id="rId2"/>
+    <sheet name="Change" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
   <si>
     <t>D</t>
   </si>
@@ -57,6 +59,12 @@
   </si>
   <si>
     <t>MOST</t>
+  </si>
+  <si>
+    <t>Least</t>
+  </si>
+  <si>
+    <t>Change</t>
   </si>
 </sst>
 </file>
@@ -101,10 +109,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,7 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EC1685A-E9BE-45D9-B98D-095FA872D69A}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
@@ -1067,4 +1077,1492 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E02F5D-CD5E-43E4-BE66-FD9721C90867}">
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>19</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>16</v>
+      </c>
+      <c r="E8">
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>14</v>
+      </c>
+      <c r="G9">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>15</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>9.5</v>
+      </c>
+      <c r="D11">
+        <v>11.5</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>13</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>12.5</v>
+      </c>
+      <c r="C13">
+        <v>8.5</v>
+      </c>
+      <c r="D13">
+        <v>10.5</v>
+      </c>
+      <c r="E13">
+        <v>10.66</v>
+      </c>
+      <c r="G13">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>10.33</v>
+      </c>
+      <c r="G14">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>9.5</v>
+      </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="G15">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>6.66</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>9.5</v>
+      </c>
+      <c r="G16">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>6.33</v>
+      </c>
+      <c r="D17">
+        <v>8.5</v>
+      </c>
+      <c r="E17">
+        <v>9</v>
+      </c>
+      <c r="G17">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>8.5</v>
+      </c>
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <v>8.66</v>
+      </c>
+      <c r="G18">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3">
+        <v>5.75</v>
+      </c>
+      <c r="D19" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>8.33</v>
+      </c>
+      <c r="G19">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D20" s="2">
+        <v>7</v>
+      </c>
+      <c r="E20" s="2">
+        <v>8</v>
+      </c>
+      <c r="G20">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>5.25</v>
+      </c>
+      <c r="D21" s="2">
+        <v>6.66</v>
+      </c>
+      <c r="E21" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="G21">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>15</v>
+      </c>
+      <c r="B22" s="4">
+        <v>6</v>
+      </c>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4">
+        <v>6.5</v>
+      </c>
+      <c r="E22" s="4">
+        <v>7</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2">
+        <v>6</v>
+      </c>
+      <c r="E23" s="2">
+        <v>6</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>17</v>
+      </c>
+      <c r="B24" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="C24" s="2">
+        <v>3.75</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4</v>
+      </c>
+      <c r="C25" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="D25" s="2">
+        <v>5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="D26" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>3</v>
+      </c>
+      <c r="D27" s="2">
+        <v>4</v>
+      </c>
+      <c r="E27" s="2">
+        <v>4</v>
+      </c>
+      <c r="G27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2.75</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.66</v>
+      </c>
+      <c r="D28" s="2">
+        <v>3.66</v>
+      </c>
+      <c r="E28" s="2">
+        <v>3.66</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2.33</v>
+      </c>
+      <c r="D29" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="E29" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="G30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="E31" s="2">
+        <v>2.75</v>
+      </c>
+      <c r="G31">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D32" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="G32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="E33" s="2">
+        <v>2.25</v>
+      </c>
+      <c r="G33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>27</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="G34">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>28</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35">
+        <v>1.66</v>
+      </c>
+      <c r="G35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>29</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D36">
+        <v>1.5</v>
+      </c>
+      <c r="E36">
+        <v>1.33</v>
+      </c>
+      <c r="G36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" s="2">
+        <v>-0.05</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38" s="2">
+        <v>0</v>
+      </c>
+      <c r="C38">
+        <v>-1</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F1D6B1-F1B9-445A-809B-308096155A80}">
+  <dimension ref="A1:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-20</v>
+      </c>
+      <c r="E2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-18</v>
+      </c>
+      <c r="E3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>-18</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>-22</v>
+      </c>
+      <c r="E5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>-21</v>
+      </c>
+      <c r="C7">
+        <v>-19</v>
+      </c>
+      <c r="D7">
+        <v>-18</v>
+      </c>
+      <c r="E7">
+        <v>-22</v>
+      </c>
+      <c r="G7">
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>-20</v>
+      </c>
+      <c r="C8">
+        <v>-18</v>
+      </c>
+      <c r="D8">
+        <v>-15</v>
+      </c>
+      <c r="E8">
+        <v>-19</v>
+      </c>
+      <c r="G8">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>-16</v>
+      </c>
+      <c r="C9">
+        <v>-10</v>
+      </c>
+      <c r="D9">
+        <v>-12.5</v>
+      </c>
+      <c r="E9">
+        <v>-15</v>
+      </c>
+      <c r="G9">
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>-14</v>
+      </c>
+      <c r="C10">
+        <v>-9</v>
+      </c>
+      <c r="D10">
+        <v>-10</v>
+      </c>
+      <c r="E10">
+        <v>-13</v>
+      </c>
+      <c r="G10">
+        <v>-13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>-12</v>
+      </c>
+      <c r="C11">
+        <v>-8</v>
+      </c>
+      <c r="D11">
+        <v>-9.66</v>
+      </c>
+      <c r="E11">
+        <v>-10</v>
+      </c>
+      <c r="G11">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>-11</v>
+      </c>
+      <c r="C12">
+        <v>-7.5</v>
+      </c>
+      <c r="D12">
+        <v>-9.33</v>
+      </c>
+      <c r="E12">
+        <v>-9.5</v>
+      </c>
+      <c r="G12">
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>-10.5</v>
+      </c>
+      <c r="C13">
+        <v>-7</v>
+      </c>
+      <c r="D13">
+        <v>-9</v>
+      </c>
+      <c r="E13">
+        <v>-9</v>
+      </c>
+      <c r="G13">
+        <v>-10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>-10</v>
+      </c>
+      <c r="C14">
+        <v>-6</v>
+      </c>
+      <c r="D14">
+        <v>-8</v>
+      </c>
+      <c r="E14">
+        <v>-8</v>
+      </c>
+      <c r="G14">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15">
+        <v>-9.66</v>
+      </c>
+      <c r="C15">
+        <v>-5.66</v>
+      </c>
+      <c r="D15">
+        <v>-7.66</v>
+      </c>
+      <c r="E15">
+        <v>-7.66</v>
+      </c>
+      <c r="G15">
+        <v>-8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>-9.33</v>
+      </c>
+      <c r="C16">
+        <v>-5.33</v>
+      </c>
+      <c r="D16">
+        <v>-7.33</v>
+      </c>
+      <c r="E16">
+        <v>-7.33</v>
+      </c>
+      <c r="G16">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17">
+        <v>-9</v>
+      </c>
+      <c r="C17">
+        <v>-5</v>
+      </c>
+      <c r="D17">
+        <v>-7</v>
+      </c>
+      <c r="E17">
+        <v>-7</v>
+      </c>
+      <c r="G17">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18">
+        <v>-7</v>
+      </c>
+      <c r="C18">
+        <v>-4</v>
+      </c>
+      <c r="D18">
+        <v>-6</v>
+      </c>
+      <c r="E18">
+        <v>-6</v>
+      </c>
+      <c r="G18">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
+        <v>-6</v>
+      </c>
+      <c r="C19" s="3">
+        <v>-3.5</v>
+      </c>
+      <c r="D19" s="2">
+        <v>-6.5</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-5</v>
+      </c>
+      <c r="G19">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" s="2">
+        <v>-5</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>-5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>-4.75</v>
+      </c>
+      <c r="G20">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" s="2">
+        <v>-4</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>-4</v>
+      </c>
+      <c r="E21" s="2">
+        <v>-4.5</v>
+      </c>
+      <c r="G21">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2">
+        <v>-3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>-1.66</v>
+      </c>
+      <c r="D22" s="2">
+        <v>-3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>-4.25</v>
+      </c>
+      <c r="G22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" s="2">
+        <v>-2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>-1.33</v>
+      </c>
+      <c r="D23" s="2">
+        <v>-2</v>
+      </c>
+      <c r="E23" s="2">
+        <v>-4</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>17</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D24" s="4">
+        <v>-1</v>
+      </c>
+      <c r="E24" s="4">
+        <v>-3</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
+      </c>
+      <c r="D25" s="2">
+        <v>-0.5</v>
+      </c>
+      <c r="E25" s="2">
+        <v>-2</v>
+      </c>
+      <c r="G25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>-1</v>
+      </c>
+      <c r="G26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>21</v>
+      </c>
+      <c r="B28" s="2">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.33</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="G28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>22</v>
+      </c>
+      <c r="B29" s="2">
+        <v>7</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2.66</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.66</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3</v>
+      </c>
+      <c r="D30" s="2">
+        <v>3</v>
+      </c>
+      <c r="E30" s="2">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="G31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>25</v>
+      </c>
+      <c r="B32" s="2">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2">
+        <v>4</v>
+      </c>
+      <c r="D32" s="2">
+        <v>5</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2</v>
+      </c>
+      <c r="G32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>26</v>
+      </c>
+      <c r="B33" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2">
+        <v>6</v>
+      </c>
+      <c r="E33" s="2">
+        <v>3</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>27</v>
+      </c>
+      <c r="B34" s="2">
+        <v>10</v>
+      </c>
+      <c r="C34" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="D34" s="2">
+        <v>7</v>
+      </c>
+      <c r="E34" s="2">
+        <v>3.33</v>
+      </c>
+      <c r="G34">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>28</v>
+      </c>
+      <c r="B35" s="2">
+        <v>12</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2">
+        <v>8</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3.66</v>
+      </c>
+      <c r="G35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>29</v>
+      </c>
+      <c r="B36" s="2">
+        <v>13</v>
+      </c>
+      <c r="C36" s="2">
+        <v>7</v>
+      </c>
+      <c r="D36" s="2">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2">
+        <v>4</v>
+      </c>
+      <c r="G36">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>30</v>
+      </c>
+      <c r="B37" s="2">
+        <v>14</v>
+      </c>
+      <c r="C37" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="D37" s="2">
+        <v>10</v>
+      </c>
+      <c r="E37" s="2">
+        <v>5</v>
+      </c>
+      <c r="G37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>31</v>
+      </c>
+      <c r="B38" s="2">
+        <v>15</v>
+      </c>
+      <c r="C38">
+        <v>8</v>
+      </c>
+      <c r="D38" s="2">
+        <v>11</v>
+      </c>
+      <c r="E38" s="2">
+        <v>6</v>
+      </c>
+      <c r="G38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>32</v>
+      </c>
+      <c r="B39" s="2">
+        <v>18</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39" s="2">
+        <v>15</v>
+      </c>
+      <c r="E39" s="2">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>33</v>
+      </c>
+      <c r="B40" s="2">
+        <v>21</v>
+      </c>
+      <c r="C40">
+        <v>18</v>
+      </c>
+      <c r="D40" s="2">
+        <v>20</v>
+      </c>
+      <c r="E40" s="2">
+        <v>17</v>
+      </c>
+      <c r="G40">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>